<commit_message>
First half first draft first chapter - 10 May
</commit_message>
<xml_diff>
--- a/Functional Diversity/trait_matrix.xlsx
+++ b/Functional Diversity/trait_matrix.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="132">
   <si>
     <t xml:space="preserve">order</t>
   </si>
@@ -410,6 +410,12 @@
   </si>
   <si>
     <t xml:space="preserve">Vanellus chilensis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rollandia rolland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sterna vittata</t>
   </si>
 </sst>
 </file>
@@ -466,13 +472,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFFFFF66"/>
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF66"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
@@ -511,7 +517,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -529,6 +535,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -621,42 +631,40 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:80"/>
+  <dimension ref="1:82"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="7912" ySplit="1410" topLeftCell="N28" activePane="bottomLeft" state="split"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="N1" activeCellId="0" sqref="N1"/>
-      <selection pane="bottomLeft" activeCell="B40" activeCellId="0" sqref="B40"/>
-      <selection pane="bottomRight" activeCell="N28" activeCellId="0" sqref="N28"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="8947" ySplit="1680" topLeftCell="A70" activePane="bottomLeft" state="split"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="F82" activeCellId="0" sqref="F82"/>
+      <selection pane="bottomRight" activeCell="A70" activeCellId="0" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.0816326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.0816326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="9.17857142857143"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
     <col collapsed="false" hidden="false" max="9" min="8" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.58673469387755"/>
     <col collapsed="false" hidden="false" max="12" min="11" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="9.31632653061224"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="4.99489795918367"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="4.86224489795918"/>
     <col collapsed="false" hidden="false" max="22" min="18" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="3.91326530612245"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="6.3469387755102"/>
     <col collapsed="false" hidden="false" max="26" min="26" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="10.8010204081633"/>
     <col collapsed="false" hidden="false" max="29" min="29" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="33" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -847,7 +855,9 @@
       <c r="R3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="S3" s="5"/>
+      <c r="S3" s="5" t="n">
+        <v>1</v>
+      </c>
       <c r="AA3" s="0" t="n">
         <v>1</v>
       </c>
@@ -1138,7 +1148,9 @@
         <v>1</v>
       </c>
       <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
+      <c r="T9" s="5" t="n">
+        <v>1</v>
+      </c>
       <c r="W9" s="0" t="n">
         <v>1</v>
       </c>
@@ -1183,7 +1195,9 @@
       <c r="R10" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="S10" s="5"/>
+      <c r="S10" s="5" t="n">
+        <v>1</v>
+      </c>
       <c r="T10" s="0" t="n">
         <v>1</v>
       </c>
@@ -1266,7 +1280,9 @@
         <v>1</v>
       </c>
       <c r="S12" s="5"/>
-      <c r="T12" s="5"/>
+      <c r="T12" s="5" t="n">
+        <v>1</v>
+      </c>
       <c r="X12" s="0" t="n">
         <v>1</v>
       </c>
@@ -1326,7 +1342,9 @@
       <c r="R13" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="S13" s="5"/>
+      <c r="S13" s="5" t="n">
+        <v>1</v>
+      </c>
       <c r="T13" s="5"/>
       <c r="W13" s="0" t="n">
         <v>1</v>
@@ -1393,7 +1411,9 @@
       <c r="R14" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="S14" s="5"/>
+      <c r="S14" s="5" t="n">
+        <v>1</v>
+      </c>
       <c r="T14" s="0" t="n">
         <v>1</v>
       </c>
@@ -2512,20 +2532,20 @@
       <c r="G39" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="H39" s="5"/>
-      <c r="I39" s="5"/>
-      <c r="J39" s="5"/>
-      <c r="K39" s="5"/>
-      <c r="L39" s="5"/>
-      <c r="M39" s="5"/>
-      <c r="N39" s="5"/>
-      <c r="O39" s="5"/>
-      <c r="P39" s="5"/>
-      <c r="Q39" s="5"/>
-      <c r="R39" s="5"/>
-      <c r="S39" s="5"/>
-      <c r="T39" s="5"/>
-      <c r="U39" s="5"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="7"/>
+      <c r="L39" s="7"/>
+      <c r="M39" s="7"/>
+      <c r="N39" s="7"/>
+      <c r="O39" s="7"/>
+      <c r="P39" s="7"/>
+      <c r="Q39" s="7"/>
+      <c r="R39" s="7"/>
+      <c r="S39" s="7"/>
+      <c r="T39" s="7"/>
+      <c r="U39" s="7"/>
       <c r="X39" s="0" t="n">
         <v>1</v>
       </c>
@@ -2596,7 +2616,7 @@
       <c r="C41" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D41" s="7" t="n">
+      <c r="D41" s="8" t="n">
         <v>609.5</v>
       </c>
       <c r="E41" s="0" t="n">
@@ -2652,7 +2672,7 @@
       <c r="C42" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D42" s="7" t="n">
+      <c r="D42" s="8" t="n">
         <v>217.5</v>
       </c>
       <c r="E42" s="0" t="n">
@@ -3072,7 +3092,7 @@
       <c r="C51" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D51" s="7" t="n">
+      <c r="D51" s="8" t="n">
         <v>75.5</v>
       </c>
       <c r="E51" s="0" t="n">
@@ -3484,7 +3504,7 @@
       <c r="C61" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D61" s="7" t="n">
+      <c r="D61" s="8" t="n">
         <v>158</v>
       </c>
       <c r="E61" s="0" t="n">
@@ -4022,7 +4042,7 @@
       <c r="C74" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D74" s="5"/>
+      <c r="D74" s="7"/>
       <c r="E74" s="0" t="n">
         <v>142</v>
       </c>
@@ -4287,7 +4307,7 @@
       <c r="C80" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D80" s="7" t="n">
+      <c r="D80" s="8" t="n">
         <v>381.5</v>
       </c>
       <c r="E80" s="0" t="n">
@@ -4321,6 +4341,92 @@
         <v>1</v>
       </c>
       <c r="AB80" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C81" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D81" s="0" t="n">
+        <v>336</v>
+      </c>
+      <c r="E81" s="7"/>
+      <c r="F81" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="G81" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="H81" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J81" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O81" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD81" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE81" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH81" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C82" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="D82" s="0" t="n">
+        <v>165</v>
+      </c>
+      <c r="E82" s="5" t="n">
+        <v>35.9</v>
+      </c>
+      <c r="F82" s="5" t="n">
+        <v>18.6</v>
+      </c>
+      <c r="G82" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="H82" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J82" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K82" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M82" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O82" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S82" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="W82" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE82" s="0" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>